<commit_message>
content header (bad position)
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Nicolas d' Haese</t>
   </si>
@@ -44,6 +44,21 @@
   </si>
   <si>
     <t>Doit pour vente</t>
+  </si>
+  <si>
+    <t>Désignation</t>
+  </si>
+  <si>
+    <t>Quantité</t>
+  </si>
+  <si>
+    <t>P.U. TVAC</t>
+  </si>
+  <si>
+    <t>Total TVAC</t>
+  </si>
+  <si>
+    <t>Code TVA</t>
   </si>
 </sst>
 </file>
@@ -449,10 +464,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:I18"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="8" max="8" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.25">
@@ -523,6 +539,23 @@
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="18" ht="30" customHeight="1" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bills order content missing
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -28,19 +28,19 @@
     <t>TVA : BE 0828.429.389            Mail : contact@dhaese-nicolas.be</t>
   </si>
   <si>
-    <t>Nom</t>
-  </si>
-  <si>
-    <t>rue</t>
-  </si>
-  <si>
-    <t>CP          COMMUNE</t>
-  </si>
-  <si>
-    <t>Bois de Lessines, date</t>
-  </si>
-  <si>
-    <t>Facture n°aa-xxx</t>
+    <t>Lol</t>
+  </si>
+  <si>
+    <t>rue de la loge 38</t>
+  </si>
+  <si>
+    <t>7866          Bois de Lessines</t>
+  </si>
+  <si>
+    <t>Bois de Lessines, 20/11/2023</t>
+  </si>
+  <si>
+    <t>Facture n°23-002</t>
   </si>
   <si>
     <t>Doit pour vente</t>

</xml_diff>